<commit_message>
Added utilities file for model
</commit_message>
<xml_diff>
--- a/data_collection/data_files/~Data tracker.xlsx
+++ b/data_collection/data_files/~Data tracker.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27421"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{64A63C8C-DECF-408F-BA27-6E6F9A8C4FC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\gmitchjr\Academic\CAPP_122\git-Planet-Status-Code-404\Final-Project\data_collection\data_files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5009A15-FDF2-4D80-8892-099AC904A172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12804" yWindow="696" windowWidth="10092" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,10 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="187">
-  <si>
-    <t>JSON Variable</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="187">
   <si>
     <t>Description</t>
   </si>
@@ -43,9 +45,6 @@
     <t>Section</t>
   </si>
   <si>
-    <t>Column1</t>
-  </si>
-  <si>
     <t>P_ENGLISH</t>
   </si>
   <si>
@@ -593,13 +592,19 @@
   </si>
   <si>
     <t>Estimated Fire Risk in 30 Years</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>JSON_Variable</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -614,8 +619,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -634,8 +647,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -643,15 +662,55 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -673,10 +732,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B9A37E71-F706-4ADD-A9BB-BDC00341A1C5}" name="Table1" displayName="Table1" ref="A1:D92" totalsRowShown="0">
   <autoFilter ref="A1:D92" xr:uid="{B9A37E71-F706-4ADD-A9BB-BDC00341A1C5}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{0EEC1FA6-53C8-4E28-941B-0ACC5E7270E8}" name="JSON Variable"/>
+    <tableColumn id="1" xr3:uid="{0EEC1FA6-53C8-4E28-941B-0ACC5E7270E8}" name="JSON_Variable"/>
     <tableColumn id="2" xr3:uid="{CEB535A9-8413-483C-A39B-7B0398A2BDB0}" name="Description"/>
     <tableColumn id="3" xr3:uid="{CFFAD15D-C4AA-4A40-A98B-0287BB0E1153}" name="Section"/>
-    <tableColumn id="4" xr3:uid="{F53D3E68-F72C-4D47-AF19-2F519111A9ED}" name="Column1"/>
+    <tableColumn id="4" xr3:uid="{F53D3E68-F72C-4D47-AF19-2F519111A9ED}" name="Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -979,12 +1038,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>185</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -993,1033 +1069,1033 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFAE12B1-48D0-4CF3-91AC-FF4954E87BB4}">
   <dimension ref="A1:D92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:XFD35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" customWidth="1"/>
+    <col min="1" max="1" width="28.88671875" customWidth="1"/>
     <col min="2" max="2" width="60" customWidth="1"/>
-    <col min="3" max="3" width="41.7109375" customWidth="1"/>
+    <col min="3" max="3" width="41.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" s="1" customFormat="1">
-      <c r="A3" s="1" t="s">
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="1" customFormat="1">
-      <c r="A4" s="1" t="s">
+      <c r="C4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="1" customFormat="1">
-      <c r="A5" s="1" t="s">
+      <c r="C5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="1" customFormat="1">
-      <c r="A6" s="1" t="s">
+      <c r="C6" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="1" customFormat="1">
-      <c r="A7" s="1" t="s">
+      <c r="C7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="1" customFormat="1">
-      <c r="A8" s="1" t="s">
+      <c r="C8" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="1" customFormat="1">
-      <c r="A9" s="1" t="s">
+      <c r="C9" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="1" customFormat="1">
-      <c r="A10" s="1" t="s">
+      <c r="C10" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="2" customFormat="1">
-      <c r="A12" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="2" t="s">
+    </row>
+    <row r="13" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" s="2" customFormat="1">
-      <c r="A13" s="2" t="s">
+      <c r="C13" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="2" customFormat="1">
-      <c r="A14" s="2" t="s">
+      <c r="C14" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" s="2" customFormat="1">
-      <c r="A15" s="2" t="s">
+      <c r="C15" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" s="2" customFormat="1">
-      <c r="A16" s="2" t="s">
+      <c r="C16" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" s="2" customFormat="1">
-      <c r="A17" s="2" t="s">
+      <c r="C17" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" s="2" customFormat="1">
-      <c r="A18" s="2" t="s">
+      <c r="C18" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" s="2" customFormat="1">
-      <c r="A19" s="2" t="s">
+      <c r="C19" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" s="1" customFormat="1">
-      <c r="A20" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="1" t="s">
+    </row>
+    <row r="21" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" s="1" customFormat="1">
-      <c r="A21" s="1" t="s">
+      <c r="C21" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" s="1" customFormat="1">
-      <c r="A22" s="1" t="s">
+      <c r="C22" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" s="1" customFormat="1">
-      <c r="A23" s="1" t="s">
+      <c r="C23" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" s="1" customFormat="1">
-      <c r="A24" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B24" s="1" t="s">
+    </row>
+    <row r="25" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" s="1" customFormat="1">
-      <c r="A25" s="1" t="s">
+      <c r="C25" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" s="1" customFormat="1">
-      <c r="A26" s="1" t="s">
+      <c r="C26" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B27" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" t="s">
+      <c r="C27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>58</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>59</v>
       </c>
-      <c r="C27" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" t="s">
+      <c r="C28" t="s">
         <v>60</v>
       </c>
-      <c r="B28" t="s">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>61</v>
       </c>
-      <c r="C28" t="s">
+      <c r="B29" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" t="s">
+      <c r="C29" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>63</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>64</v>
       </c>
-      <c r="C29" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" t="s">
+      <c r="C30" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>65</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>66</v>
       </c>
-      <c r="C30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" t="s">
+      <c r="C31" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>67</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>68</v>
       </c>
-      <c r="C31" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" t="s">
+      <c r="C32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>69</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>70</v>
       </c>
-      <c r="C32" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" t="s">
+      <c r="C33" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C33" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" s="1" customFormat="1">
-      <c r="A34" s="1" t="s">
+      <c r="C34" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" s="1" customFormat="1">
-      <c r="A35" s="1" t="s">
+      <c r="C35" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>75</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B36" t="s">
         <v>76</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" t="s">
+      <c r="C36" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>77</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>78</v>
       </c>
-      <c r="C36" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" t="s">
+      <c r="C37" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>79</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>80</v>
       </c>
-      <c r="C37" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" t="s">
+      <c r="C38" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>81</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>82</v>
       </c>
-      <c r="C38" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" t="s">
+      <c r="C39" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>83</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>84</v>
       </c>
-      <c r="C39" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" t="s">
+      <c r="C40" t="s">
         <v>85</v>
       </c>
-      <c r="B40" t="s">
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>86</v>
       </c>
-      <c r="C40" t="s">
+      <c r="B41" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" t="s">
+      <c r="C41" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>88</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>89</v>
       </c>
-      <c r="C41" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" t="s">
+      <c r="C42" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>90</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>91</v>
       </c>
-      <c r="C42" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" t="s">
+      <c r="C43" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>92</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>93</v>
       </c>
-      <c r="C43" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" t="s">
+      <c r="C44" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>94</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>95</v>
       </c>
-      <c r="C44" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" t="s">
+      <c r="C45" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C45" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" s="3" customFormat="1">
-      <c r="A46" s="3" t="s">
+      <c r="C46" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D46" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B46" s="3" t="s">
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>99</v>
       </c>
-      <c r="C46" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D46" s="3" t="s">
+      <c r="B47" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" t="s">
+      <c r="C47" t="s">
         <v>101</v>
       </c>
-      <c r="B47" t="s">
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>102</v>
       </c>
-      <c r="C47" t="s">
+      <c r="B48" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" t="s">
+      <c r="C48" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>104</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>105</v>
       </c>
-      <c r="C48" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" t="s">
+      <c r="C49" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C49" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" s="1" customFormat="1">
-      <c r="A50" s="1" t="s">
+      <c r="C50" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" s="1" customFormat="1">
-      <c r="A51" s="1" t="s">
+      <c r="C51" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B52" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" s="1" customFormat="1">
-      <c r="A52" s="1" t="s">
+      <c r="C52" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>112</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B53" t="s">
         <v>113</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" t="s">
+      <c r="C53" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>114</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B54" t="s">
         <v>115</v>
       </c>
-      <c r="C53" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" t="s">
+      <c r="C54" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C54" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" s="1" customFormat="1">
-      <c r="A55" s="1" t="s">
+      <c r="C55" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
         <v>118</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B56" t="s">
         <v>119</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" t="s">
+      <c r="C56" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
         <v>120</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>121</v>
       </c>
-      <c r="C56" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" t="s">
-        <v>122</v>
-      </c>
-      <c r="B57" t="s">
+      <c r="C57" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
         <v>123</v>
       </c>
-      <c r="C57" t="s">
+      <c r="B58" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" t="s">
+      <c r="C58" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B59" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C58" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" s="1" customFormat="1">
-      <c r="A59" s="1" t="s">
+      <c r="C59" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
         <v>127</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B60" t="s">
         <v>128</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" t="s">
+      <c r="C60" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B61" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C60" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" s="1" customFormat="1">
-      <c r="A61" s="1" t="s">
+      <c r="C61" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B62" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" s="1" customFormat="1">
-      <c r="A62" s="1" t="s">
+      <c r="C62" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B63" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" s="1" customFormat="1">
-      <c r="A63" s="1" t="s">
+      <c r="C63" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
         <v>135</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B64" t="s">
         <v>136</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="A64" t="s">
+      <c r="C64" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
         <v>137</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B65" t="s">
         <v>138</v>
       </c>
-      <c r="C64" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65" t="s">
+      <c r="C65" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B66" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C65" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" s="1" customFormat="1">
-      <c r="A66" s="1" t="s">
+      <c r="C66" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B67" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C66" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" s="1" customFormat="1">
-      <c r="A67" s="1" t="s">
+      <c r="C67" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
         <v>143</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B68" t="s">
         <v>144</v>
       </c>
-      <c r="C67" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="A68" t="s">
+      <c r="C68" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B69" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C68" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" s="1" customFormat="1">
-      <c r="A69" s="1" t="s">
+      <c r="C69" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B70" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C69" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" s="1" customFormat="1">
-      <c r="A70" s="1" t="s">
+      <c r="C70" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B71" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C70" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" s="1" customFormat="1">
-      <c r="A71" s="1" t="s">
+      <c r="B72" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
         <v>151</v>
       </c>
-      <c r="B71" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" s="1" customFormat="1">
-      <c r="A72" s="1" t="s">
+      <c r="B73" t="s">
+        <v>148</v>
+      </c>
+      <c r="C73" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
         <v>152</v>
       </c>
-      <c r="B72" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="A73" t="s">
+      <c r="B74" t="s">
+        <v>148</v>
+      </c>
+      <c r="C74" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
         <v>153</v>
       </c>
-      <c r="B73" t="s">
-        <v>150</v>
-      </c>
-      <c r="C73" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74" t="s">
+      <c r="B75" t="s">
+        <v>148</v>
+      </c>
+      <c r="C75" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B74" t="s">
-        <v>150</v>
-      </c>
-      <c r="C74" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="A75" t="s">
+      <c r="B76" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
         <v>155</v>
       </c>
-      <c r="B75" t="s">
-        <v>150</v>
-      </c>
-      <c r="C75" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" s="1" customFormat="1">
-      <c r="A76" s="1" t="s">
+      <c r="B77" t="s">
+        <v>148</v>
+      </c>
+      <c r="C77" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
         <v>156</v>
       </c>
-      <c r="B76" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="A77" t="s">
+      <c r="B78" t="s">
+        <v>148</v>
+      </c>
+      <c r="C78" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
         <v>157</v>
       </c>
-      <c r="B77" t="s">
-        <v>150</v>
-      </c>
-      <c r="C77" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3">
-      <c r="A78" t="s">
+      <c r="B79" t="s">
+        <v>148</v>
+      </c>
+      <c r="C79" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
         <v>158</v>
       </c>
-      <c r="B78" t="s">
-        <v>150</v>
-      </c>
-      <c r="C78" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3">
-      <c r="A79" t="s">
+      <c r="B80" t="s">
+        <v>148</v>
+      </c>
+      <c r="C80" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
         <v>159</v>
       </c>
-      <c r="B79" t="s">
-        <v>150</v>
-      </c>
-      <c r="C79" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3">
-      <c r="A80" t="s">
+      <c r="B81" t="s">
+        <v>148</v>
+      </c>
+      <c r="C81" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
         <v>160</v>
       </c>
-      <c r="B80" t="s">
-        <v>150</v>
-      </c>
-      <c r="C80" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3">
-      <c r="A81" t="s">
+      <c r="B82" t="s">
         <v>161</v>
       </c>
-      <c r="B81" t="s">
-        <v>150</v>
-      </c>
-      <c r="C81" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3">
-      <c r="A82" t="s">
+      <c r="C82" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
         <v>162</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B83" t="s">
         <v>163</v>
       </c>
-      <c r="C82" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3">
-      <c r="A83" t="s">
+      <c r="C83" t="s">
         <v>164</v>
       </c>
-      <c r="B83" t="s">
+    </row>
+    <row r="84" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="C83" t="s">
+      <c r="B84" s="1" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" s="1" customFormat="1">
-      <c r="A84" s="1" t="s">
+      <c r="C84" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
         <v>167</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B85" t="s">
         <v>168</v>
       </c>
-      <c r="C84" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3">
-      <c r="A85" t="s">
+      <c r="C85" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B86" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C85" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" s="1" customFormat="1">
-      <c r="A86" s="1" t="s">
+      <c r="C86" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
         <v>171</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="B87" t="s">
         <v>172</v>
       </c>
-      <c r="C86" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3">
-      <c r="A87" t="s">
+      <c r="C87" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
         <v>173</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B88" t="s">
         <v>174</v>
       </c>
-      <c r="C87" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3">
-      <c r="A88" t="s">
+      <c r="C88" t="s">
         <v>175</v>
       </c>
-      <c r="B88" t="s">
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
         <v>176</v>
       </c>
-      <c r="C88" t="s">
+      <c r="B89" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="89" spans="1:3">
-      <c r="A89" t="s">
+      <c r="C89" t="s">
         <v>178</v>
       </c>
-      <c r="B89" t="s">
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
         <v>179</v>
       </c>
-      <c r="C89" t="s">
+      <c r="B90" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="90" spans="1:3">
-      <c r="A90" t="s">
+      <c r="C90" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
         <v>181</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B91" t="s">
         <v>182</v>
       </c>
-      <c r="C90" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3">
-      <c r="A91" t="s">
+      <c r="C91" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
         <v>183</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B92" t="s">
         <v>184</v>
       </c>
-      <c r="C91" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3">
-      <c r="A92" t="s">
-        <v>185</v>
-      </c>
-      <c r="B92" t="s">
-        <v>186</v>
-      </c>
       <c r="C92" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>